<commit_message>
PI45 goes to PIP3
</commit_message>
<xml_diff>
--- a/mtor/mTOR56.xlsx
+++ b/mtor/mTOR56.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yassenroussev/Desktop/mTOR/mtor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318AEDF8-E2C9-F14A-B839-F39E5C447BEB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2FE645-9F08-114B-88CF-E9FA955EEE8D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="256">
   <si>
     <t>!!SBtab TableType='rxnconReactionList' TableName='ReactionList'</t>
   </si>
@@ -843,7 +843,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -973,6 +973,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1114,7 +1120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1234,6 +1240,8 @@
     <xf numFmtId="0" fontId="4" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4170,10 +4178,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV149"/>
+  <dimension ref="A1:IV148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="139" zoomScaleSheetLayoutView="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
@@ -4419,14 +4427,14 @@
       <c r="A14" s="12">
         <v>7</v>
       </c>
-      <c r="B14" s="41" t="str">
+      <c r="B14" s="71" t="str">
         <f>ReactionList!A11</f>
         <v>PI3K_p+_PI_[(3)]</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="71" t="s">
         <v>96</v>
       </c>
       <c r="E14" s="37" t="s">
@@ -4439,14 +4447,14 @@
       <c r="A15" s="12">
         <v>10</v>
       </c>
-      <c r="B15" s="41" t="str">
+      <c r="B15" s="71" t="str">
         <f>ReactionList!A13</f>
         <v>AKT2_[PI]_i_PI_[PH]</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="72" t="s">
         <v>100</v>
       </c>
       <c r="E15" s="37"/>
@@ -4457,14 +4465,14 @@
       <c r="A16" s="12">
         <v>11</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="41" t="s">
-        <v>99</v>
+      <c r="D16" s="72" t="s">
+        <v>255</v>
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
@@ -4472,16 +4480,16 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="12">
-        <v>12</v>
-      </c>
-      <c r="B17" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="D17" s="41" t="s">
-        <v>98</v>
+      <c r="D17" s="71" t="s">
+        <v>102</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="37"/>
@@ -4489,16 +4497,17 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="12">
-        <v>13</v>
-      </c>
-      <c r="B18" s="41" t="s">
-        <v>100</v>
+        <v>14</v>
+      </c>
+      <c r="B18" s="41" t="str">
+        <f>ReactionList!A14</f>
+        <v>PDK1_p+_AKT2_[(T309)]</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="D18" s="41" t="s">
-        <v>102</v>
+        <v>87</v>
+      </c>
+      <c r="D18" s="53" t="s">
+        <v>103</v>
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="37"/>
@@ -4506,11 +4515,11 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19" s="41" t="str">
-        <f>ReactionList!A14</f>
-        <v>PDK1_p+_AKT2_[(T309)]</v>
+        <f>ReactionList!A15</f>
+        <v>mTORC2_p+_AKT2_[(S474)]</v>
       </c>
       <c r="C19" s="41" t="s">
         <v>87</v>
@@ -4524,17 +4533,17 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="12">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B20" s="41" t="str">
-        <f>ReactionList!A15</f>
-        <v>mTORC2_p+_AKT2_[(S474)]</v>
+        <f>ReactionList!A18</f>
+        <v>AKT2_p+_TSC2_[(Ser939)]</v>
       </c>
       <c r="C20" s="41" t="s">
         <v>87</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="37"/>
@@ -4542,11 +4551,11 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="12">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B21" s="41" t="str">
-        <f>ReactionList!A18</f>
-        <v>AKT2_p+_TSC2_[(Ser939)]</v>
+        <f>ReactionList!A19</f>
+        <v>AKT2_p+_TSC2_[(Thr1462)]</v>
       </c>
       <c r="C21" s="41" t="s">
         <v>87</v>
@@ -4560,11 +4569,11 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="12">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B22" s="41" t="str">
-        <f>ReactionList!A19</f>
-        <v>AKT2_p+_TSC2_[(Thr1462)]</v>
+        <f>ReactionList!A20</f>
+        <v>AKT2_p+_TSC2_[(Ser981)]</v>
       </c>
       <c r="C22" s="41" t="s">
         <v>87</v>
@@ -4578,11 +4587,11 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="12">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B23" s="41" t="str">
-        <f>ReactionList!A20</f>
-        <v>AKT2_p+_TSC2_[(Ser981)]</v>
+        <f>ReactionList!A21</f>
+        <v>AKT2_p+_TSC2_[(Ser1130)]</v>
       </c>
       <c r="C23" s="41" t="s">
         <v>87</v>
@@ -4595,31 +4604,29 @@
       <c r="G23" s="33"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="12">
-        <v>19</v>
-      </c>
-      <c r="B24" s="41" t="str">
-        <f>ReactionList!A21</f>
-        <v>AKT2_p+_TSC2_[(Ser1130)]</v>
-      </c>
-      <c r="C24" s="41" t="s">
+      <c r="A24" s="12"/>
+      <c r="B24" s="61" t="str">
+        <f>ReactionList!A22</f>
+        <v>AKT2_p+_PPM1G_[(AKT2)]</v>
+      </c>
+      <c r="C24" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="53" t="s">
+      <c r="D24" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="33"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="36"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="12"/>
       <c r="B25" s="61" t="str">
-        <f>ReactionList!A22</f>
-        <v>AKT2_p+_PPM1G_[(AKT2)]</v>
+        <f>ReactionList!A23</f>
+        <v>un_p-_PPM1G_[(AKT2)]</v>
       </c>
       <c r="C25" s="61" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="D25" s="63" t="s">
         <v>104</v>
@@ -4629,24 +4636,25 @@
       <c r="G25" s="36"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="12"/>
-      <c r="B26" s="61" t="str">
-        <f>ReactionList!A23</f>
-        <v>un_p-_PPM1G_[(AKT2)]</v>
-      </c>
-      <c r="C26" s="61" t="s">
-        <v>110</v>
-      </c>
-      <c r="D26" s="63" t="s">
+      <c r="A26" s="12">
+        <v>20</v>
+      </c>
+      <c r="B26" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="36"/>
+      <c r="C26" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="12">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B27" s="53" t="s">
         <v>104</v>
@@ -4655,7 +4663,7 @@
         <v>101</v>
       </c>
       <c r="D27" s="53" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E27" s="37"/>
       <c r="F27" s="37"/>
@@ -4663,16 +4671,17 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="12">
-        <v>21</v>
-      </c>
-      <c r="B28" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="C28" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="D28" s="53" t="s">
-        <v>106</v>
+        <v>23</v>
+      </c>
+      <c r="B28" s="42" t="str">
+        <f>ReactionList!A32</f>
+        <v>RHEB_[switch1]_ppi_mTOR_[Mheatmα2mα3mα4]</v>
+      </c>
+      <c r="C28" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>107</v>
       </c>
       <c r="E28" s="37"/>
       <c r="F28" s="37"/>
@@ -4680,11 +4689,11 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="12">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B29" s="42" t="str">
-        <f>ReactionList!A32</f>
-        <v>RHEB_[switch1]_ppi_mTOR_[Mheatmα2mα3mα4]</v>
+        <f>ReactionList!A33</f>
+        <v>RHEB_[switch2GQDEYSIFPQTYSIDIN]_ppi_mTOR_[Nheatnα3tonα7]</v>
       </c>
       <c r="C29" s="55" t="s">
         <v>87</v>
@@ -4698,11 +4707,11 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="12">
-        <v>24</v>
-      </c>
-      <c r="B30" s="42" t="str">
-        <f>ReactionList!A33</f>
-        <v>RHEB_[switch2GQDEYSIFPQTYSIDIN]_ppi_mTOR_[Nheatnα3tonα7]</v>
+        <v>25</v>
+      </c>
+      <c r="B30" s="44" t="str">
+        <f>ReactionList!A34</f>
+        <v>RHEB_[switch1DSYDPTIEN]_ppi_mTOR_[FATfα2fα3]</v>
       </c>
       <c r="C30" s="55" t="s">
         <v>87</v>
@@ -4716,17 +4725,16 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="12">
-        <v>25</v>
-      </c>
-      <c r="B31" s="44" t="str">
-        <f>ReactionList!A34</f>
-        <v>RHEB_[switch1DSYDPTIEN]_ppi_mTOR_[FATfα2fα3]</v>
+        <v>26</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>108</v>
       </c>
       <c r="C31" s="55" t="s">
         <v>87</v>
       </c>
       <c r="D31" s="42" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E31" s="37"/>
       <c r="F31" s="37"/>
@@ -4734,50 +4742,51 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="12">
-        <v>26</v>
-      </c>
-      <c r="B32" s="44" t="s">
-        <v>108</v>
+        <v>27</v>
+      </c>
+      <c r="B32" s="44" t="str">
+        <f>ReactionList!A28</f>
+        <v>TSC1_[Cterminus]_ppi+_TSC2_[Nterminus]</v>
       </c>
       <c r="C32" s="55" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="D32" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" s="37"/>
+        <v>111</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>112</v>
+      </c>
       <c r="F32" s="37"/>
-      <c r="G32" s="33"/>
+      <c r="G32" s="33" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="12">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B33" s="44" t="str">
-        <f>ReactionList!A28</f>
-        <v>TSC1_[Cterminus]_ppi+_TSC2_[Nterminus]</v>
+        <f>ReactionList!A29</f>
+        <v>TSC1_[Cterminus]_ppi-_TSC2_[Nterminus]</v>
       </c>
       <c r="C33" s="55" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="D33" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="E33" s="37" t="s">
-        <v>112</v>
-      </c>
+      <c r="E33" s="37"/>
       <c r="F33" s="37"/>
-      <c r="G33" s="33" t="s">
-        <v>113</v>
-      </c>
+      <c r="G33" s="33"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="12">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B34" s="44" t="str">
-        <f>ReactionList!A29</f>
-        <v>TSC1_[Cterminus]_ppi-_TSC2_[Nterminus]</v>
+        <f>ReactionList!A30</f>
+        <v>GTP_gef_RHEB_[(G)]</v>
       </c>
       <c r="C34" s="55" t="s">
         <v>87</v>
@@ -4791,17 +4800,16 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="12">
-        <v>29</v>
-      </c>
-      <c r="B35" s="44" t="str">
-        <f>ReactionList!A30</f>
-        <v>GTP_gef_RHEB_[(G)]</v>
+        <v>30</v>
+      </c>
+      <c r="B35" s="44" t="s">
+        <v>114</v>
       </c>
       <c r="C35" s="55" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D35" s="42" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E35" s="37"/>
       <c r="F35" s="37"/>
@@ -4809,7 +4817,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="12">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B36" s="44" t="s">
         <v>114</v>
@@ -4818,7 +4826,7 @@
         <v>101</v>
       </c>
       <c r="D36" s="42" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E36" s="37"/>
       <c r="F36" s="37"/>
@@ -4826,7 +4834,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="12">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B37" s="44" t="s">
         <v>114</v>
@@ -4835,7 +4843,7 @@
         <v>101</v>
       </c>
       <c r="D37" s="42" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E37" s="37"/>
       <c r="F37" s="37"/>
@@ -4843,7 +4851,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="12">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B38" s="44" t="s">
         <v>114</v>
@@ -4852,7 +4860,7 @@
         <v>101</v>
       </c>
       <c r="D38" s="42" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E38" s="37"/>
       <c r="F38" s="37"/>
@@ -4860,24 +4868,29 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="12">
-        <v>33</v>
-      </c>
-      <c r="B39" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="C39" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="D39" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="E39" s="37"/>
+        <v>34</v>
+      </c>
+      <c r="B39" s="38" t="str">
+        <f>ReactionList!A35</f>
+        <v>mTOR_ppi+_Raptor</v>
+      </c>
+      <c r="C39" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" s="37" t="s">
+        <v>120</v>
+      </c>
       <c r="F39" s="37"/>
-      <c r="G39" s="33"/>
+      <c r="G39" s="33" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="12">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B40" s="38" t="str">
         <f>ReactionList!A35</f>
@@ -4887,43 +4900,39 @@
         <v>87</v>
       </c>
       <c r="D40" s="32" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E40" s="37" t="s">
         <v>120</v>
       </c>
       <c r="F40" s="37"/>
-      <c r="G40" s="33" t="s">
-        <v>121</v>
-      </c>
+      <c r="G40" s="33"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="12">
-        <v>35</v>
-      </c>
-      <c r="B41" s="38" t="str">
-        <f>ReactionList!A35</f>
-        <v>mTOR_ppi+_Raptor</v>
-      </c>
-      <c r="C41" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="57" t="str">
+        <f>ReactionList!A38</f>
+        <v>mTORC1_p+_EIF4EBP1_[(Thr37)]</v>
+      </c>
+      <c r="C41" s="57" t="s">
         <v>87</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="E41" s="37" t="s">
-        <v>120</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="E41" s="37"/>
       <c r="F41" s="37"/>
       <c r="G41" s="33"/>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="12">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B42" s="57" t="str">
-        <f>ReactionList!A38</f>
-        <v>mTORC1_p+_EIF4EBP1_[(Thr37)]</v>
+        <f>ReactionList!A39</f>
+        <v>mTORC1_p+_EIF4EBP1_[(Thr46)]</v>
       </c>
       <c r="C42" s="57" t="s">
         <v>87</v>
@@ -4936,12 +4945,10 @@
       <c r="G42" s="33"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="12">
-        <v>40</v>
-      </c>
+      <c r="A43" s="12"/>
       <c r="B43" s="57" t="str">
-        <f>ReactionList!A39</f>
-        <v>mTORC1_p+_EIF4EBP1_[(Thr46)]</v>
+        <f>ReactionList!A40</f>
+        <v>mTORC1_p+_EIF4EBP1_[(Ser65)]</v>
       </c>
       <c r="C43" s="57" t="s">
         <v>87</v>
@@ -4956,8 +4963,8 @@
     <row r="44" spans="1:7">
       <c r="A44" s="12"/>
       <c r="B44" s="57" t="str">
-        <f>ReactionList!A40</f>
-        <v>mTORC1_p+_EIF4EBP1_[(Ser65)]</v>
+        <f>ReactionList!A41</f>
+        <v>mTORC1_p+_EIF4EBP1_[(Thr70)]</v>
       </c>
       <c r="C44" s="57" t="s">
         <v>87</v>
@@ -4971,15 +4978,14 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="12"/>
-      <c r="B45" s="57" t="str">
-        <f>ReactionList!A41</f>
-        <v>mTORC1_p+_EIF4EBP1_[(Thr70)]</v>
+      <c r="B45" s="32" t="s">
+        <v>123</v>
       </c>
       <c r="C45" s="57" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E45" s="37"/>
       <c r="F45" s="37"/>
@@ -4993,8 +4999,8 @@
       <c r="C46" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="D46" s="32" t="s">
-        <v>124</v>
+      <c r="D46" s="46" t="s">
+        <v>125</v>
       </c>
       <c r="E46" s="37"/>
       <c r="F46" s="37"/>
@@ -5009,7 +5015,7 @@
         <v>101</v>
       </c>
       <c r="D47" s="46" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E47" s="37"/>
       <c r="F47" s="37"/>
@@ -5023,31 +5029,40 @@
       <c r="C48" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="D48" s="46" t="s">
-        <v>126</v>
+      <c r="D48" s="43" t="s">
+        <v>127</v>
       </c>
       <c r="E48" s="37"/>
       <c r="F48" s="37"/>
       <c r="G48" s="33"/>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="12"/>
-      <c r="B49" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="C49" s="57" t="s">
-        <v>101</v>
-      </c>
-      <c r="D49" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="33"/>
+      <c r="A49" s="12">
+        <v>41</v>
+      </c>
+      <c r="B49" s="35" t="str">
+        <f>ReactionList!A41</f>
+        <v>mTORC1_p+_EIF4EBP1_[(Thr70)]</v>
+      </c>
+      <c r="C49" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="F49" s="51"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="1" t="str">
+        <f>""</f>
+        <v/>
+      </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="12">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B50" s="35" t="str">
         <f>ReactionList!A41</f>
@@ -5057,31 +5072,27 @@
         <v>87</v>
       </c>
       <c r="D50" s="40" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E50" s="34" t="s">
         <v>129</v>
       </c>
       <c r="F50" s="51"/>
       <c r="G50" s="36"/>
-      <c r="H50" s="1" t="str">
-        <f>""</f>
-        <v/>
-      </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="12">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B51" s="35" t="str">
-        <f>ReactionList!A41</f>
-        <v>mTORC1_p+_EIF4EBP1_[(Thr70)]</v>
+        <f>ReactionList!A40</f>
+        <v>mTORC1_p+_EIF4EBP1_[(Ser65)]</v>
       </c>
       <c r="C51" s="35" t="s">
         <v>87</v>
       </c>
       <c r="D51" s="40" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E51" s="34" t="s">
         <v>129</v>
@@ -5091,7 +5102,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="12">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B52" s="35" t="str">
         <f>ReactionList!A40</f>
@@ -5101,7 +5112,7 @@
         <v>87</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E52" s="34" t="s">
         <v>129</v>
@@ -5111,7 +5122,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="12">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B53" s="35" t="str">
         <f>ReactionList!A40</f>
@@ -5121,7 +5132,7 @@
         <v>87</v>
       </c>
       <c r="D53" s="40" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E53" s="34" t="s">
         <v>129</v>
@@ -5131,31 +5142,29 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="12">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B54" s="35" t="str">
-        <f>ReactionList!A40</f>
-        <v>mTORC1_p+_EIF4EBP1_[(Ser65)]</v>
+        <f>ReactionList!A38</f>
+        <v>mTORC1_p+_EIF4EBP1_[(Thr37)]</v>
       </c>
       <c r="C54" s="35" t="s">
         <v>87</v>
       </c>
       <c r="D54" s="40" t="s">
-        <v>131</v>
-      </c>
-      <c r="E54" s="34" t="s">
-        <v>129</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="E54" s="34"/>
       <c r="F54" s="51"/>
       <c r="G54" s="36"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="12">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B55" s="35" t="str">
-        <f>ReactionList!A38</f>
-        <v>mTORC1_p+_EIF4EBP1_[(Thr37)]</v>
+        <f>ReactionList!A39</f>
+        <v>mTORC1_p+_EIF4EBP1_[(Thr46)]</v>
       </c>
       <c r="C55" s="35" t="s">
         <v>87</v>
@@ -5169,11 +5178,11 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="12">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B56" s="35" t="str">
-        <f>ReactionList!A39</f>
-        <v>mTORC1_p+_EIF4EBP1_[(Thr46)]</v>
+        <f>ReactionList!A41</f>
+        <v>mTORC1_p+_EIF4EBP1_[(Thr70)]</v>
       </c>
       <c r="C56" s="35" t="s">
         <v>87</v>
@@ -5187,11 +5196,11 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="12">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B57" s="35" t="str">
-        <f>ReactionList!A41</f>
-        <v>mTORC1_p+_EIF4EBP1_[(Thr70)]</v>
+        <f>ReactionList!A40</f>
+        <v>mTORC1_p+_EIF4EBP1_[(Ser65)]</v>
       </c>
       <c r="C57" s="35" t="s">
         <v>87</v>
@@ -5204,28 +5213,28 @@
       <c r="G57" s="36"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="12">
-        <v>49</v>
-      </c>
-      <c r="B58" s="35" t="str">
-        <f>ReactionList!A40</f>
-        <v>mTORC1_p+_EIF4EBP1_[(Ser65)]</v>
-      </c>
-      <c r="C58" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="D58" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="E58" s="34"/>
+      <c r="A58" s="12"/>
+      <c r="B58" s="61" t="str">
+        <f>ReactionList!A42</f>
+        <v>PPM1G_p-_EIF4EBP1_[(Thr37)]</v>
+      </c>
+      <c r="C58" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="D58" s="62" t="s">
+        <v>242</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>244</v>
+      </c>
       <c r="F58" s="51"/>
       <c r="G58" s="36"/>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="12"/>
       <c r="B59" s="61" t="str">
-        <f>ReactionList!A42</f>
-        <v>PPM1G_p-_EIF4EBP1_[(Thr37)]</v>
+        <f>ReactionList!A43</f>
+        <v>PPM1G_p-_EIF4EBP1_[(Thr46)]</v>
       </c>
       <c r="C59" s="61" t="s">
         <v>110</v>
@@ -5233,7 +5242,7 @@
       <c r="D59" s="62" t="s">
         <v>242</v>
       </c>
-      <c r="E59" s="13" t="s">
+      <c r="E59" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F59" s="51"/>
@@ -5242,8 +5251,8 @@
     <row r="60" spans="1:8">
       <c r="A60" s="12"/>
       <c r="B60" s="61" t="str">
-        <f>ReactionList!A43</f>
-        <v>PPM1G_p-_EIF4EBP1_[(Thr46)]</v>
+        <f>ReactionList!A44</f>
+        <v>PPM1G_p-_EIF4EBP1_[(Ser65)]</v>
       </c>
       <c r="C60" s="61" t="s">
         <v>110</v>
@@ -5260,8 +5269,8 @@
     <row r="61" spans="1:8">
       <c r="A61" s="12"/>
       <c r="B61" s="61" t="str">
-        <f>ReactionList!A44</f>
-        <v>PPM1G_p-_EIF4EBP1_[(Ser65)]</v>
+        <f>ReactionList!A45</f>
+        <v>PPM1G_p-_EIF4EBP1_[(Thr70)]</v>
       </c>
       <c r="C61" s="61" t="s">
         <v>110</v>
@@ -5276,36 +5285,33 @@
       <c r="G61" s="36"/>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="12"/>
-      <c r="B62" s="61" t="str">
-        <f>ReactionList!A45</f>
-        <v>PPM1G_p-_EIF4EBP1_[(Thr70)]</v>
-      </c>
-      <c r="C62" s="61" t="s">
-        <v>110</v>
-      </c>
-      <c r="D62" s="62" t="s">
-        <v>242</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>244</v>
-      </c>
+      <c r="A62" s="12">
+        <v>54</v>
+      </c>
+      <c r="B62" s="30" t="str">
+        <f>ReactionList!A37</f>
+        <v>eIF4E_[A001]_ppi-_EIF4EBP1_[A001]</v>
+      </c>
+      <c r="C62" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="E62" s="34"/>
       <c r="F62" s="51"/>
       <c r="G62" s="36"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="12">
-        <v>54</v>
-      </c>
-      <c r="B63" s="30" t="str">
-        <f>ReactionList!A37</f>
-        <v>eIF4E_[A001]_ppi-_EIF4EBP1_[A001]</v>
-      </c>
-      <c r="C63" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="D63" s="47" t="s">
-        <v>133</v>
+      <c r="A63" s="12"/>
+      <c r="B63" s="56" t="s">
+        <v>134</v>
+      </c>
+      <c r="C63" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="D63" s="31" t="s">
+        <v>135</v>
       </c>
       <c r="E63" s="34"/>
       <c r="F63" s="51"/>
@@ -5313,14 +5319,14 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="12"/>
-      <c r="B64" s="56" t="s">
+      <c r="B64" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="C64" s="56" t="s">
+      <c r="C64" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="D64" s="31" t="s">
-        <v>135</v>
+      <c r="D64" s="29" t="s">
+        <v>136</v>
       </c>
       <c r="E64" s="34"/>
       <c r="F64" s="51"/>
@@ -5335,7 +5341,7 @@
         <v>101</v>
       </c>
       <c r="D65" s="29" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E65" s="34"/>
       <c r="F65" s="51"/>
@@ -5350,7 +5356,7 @@
         <v>101</v>
       </c>
       <c r="D66" s="29" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E66" s="34"/>
       <c r="F66" s="51"/>
@@ -5358,30 +5364,32 @@
     </row>
     <row r="67" spans="1:256">
       <c r="A67" s="12"/>
-      <c r="B67" s="48" t="s">
-        <v>134</v>
-      </c>
-      <c r="C67" s="48" t="s">
-        <v>101</v>
-      </c>
-      <c r="D67" s="29" t="s">
-        <v>138</v>
+      <c r="B67" s="30" t="str">
+        <f>ReactionList!A46</f>
+        <v>eIF4E_[A001]_ppi_eIF4G_[A002]</v>
+      </c>
+      <c r="C67" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="D67" s="47" t="s">
+        <v>133</v>
       </c>
       <c r="E67" s="34"/>
       <c r="F67" s="51"/>
       <c r="G67" s="36"/>
     </row>
     <row r="68" spans="1:256">
-      <c r="A68" s="12"/>
-      <c r="B68" s="30" t="str">
-        <f>ReactionList!A46</f>
-        <v>eIF4E_[A001]_ppi_eIF4G_[A002]</v>
-      </c>
-      <c r="C68" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="D68" s="47" t="s">
-        <v>133</v>
+      <c r="A68" s="12">
+        <v>55</v>
+      </c>
+      <c r="B68" s="56" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="D68" s="31" t="s">
+        <v>135</v>
       </c>
       <c r="E68" s="34"/>
       <c r="F68" s="51"/>
@@ -5389,16 +5397,16 @@
     </row>
     <row r="69" spans="1:256">
       <c r="A69" s="12">
-        <v>55</v>
-      </c>
-      <c r="B69" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="B69" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="C69" s="56" t="s">
+      <c r="C69" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="D69" s="31" t="s">
-        <v>135</v>
+      <c r="D69" s="29" t="s">
+        <v>136</v>
       </c>
       <c r="E69" s="34"/>
       <c r="F69" s="51"/>
@@ -5406,7 +5414,7 @@
     </row>
     <row r="70" spans="1:256">
       <c r="A70" s="12">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B70" s="48" t="s">
         <v>134</v>
@@ -5415,7 +5423,7 @@
         <v>101</v>
       </c>
       <c r="D70" s="29" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E70" s="34"/>
       <c r="F70" s="51"/>
@@ -5423,7 +5431,7 @@
     </row>
     <row r="71" spans="1:256">
       <c r="A71" s="12">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B71" s="48" t="s">
         <v>134</v>
@@ -5432,61 +5440,56 @@
         <v>101</v>
       </c>
       <c r="D71" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="E71" s="34"/>
-      <c r="F71" s="51"/>
-      <c r="G71" s="36"/>
+        <v>138</v>
+      </c>
     </row>
     <row r="72" spans="1:256">
-      <c r="A72" s="12">
-        <v>58</v>
-      </c>
-      <c r="B72" s="48" t="s">
-        <v>134</v>
-      </c>
-      <c r="C72" s="48" t="s">
-        <v>101</v>
-      </c>
-      <c r="D72" s="29" t="s">
-        <v>138</v>
+      <c r="A72" s="12"/>
+      <c r="B72" s="52" t="str">
+        <f>ReactionList!A36</f>
+        <v>eIF4E_[A001]_ppi+_EIF4EBP1_[A001]</v>
+      </c>
+      <c r="C72" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="D72" s="47" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="73" spans="1:256">
       <c r="A73" s="12"/>
-      <c r="B73" s="52" t="str">
-        <f>ReactionList!A36</f>
-        <v>eIF4E_[A001]_ppi+_EIF4EBP1_[A001]</v>
+      <c r="B73" s="50" t="s">
+        <v>134</v>
       </c>
       <c r="C73" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="D73" s="47" t="s">
-        <v>133</v>
+        <v>101</v>
+      </c>
+      <c r="D73" s="31" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:256">
       <c r="A74" s="12"/>
-      <c r="B74" s="50" t="s">
+      <c r="B74" s="56" t="s">
         <v>134</v>
       </c>
-      <c r="C74" s="49" t="s">
+      <c r="C74" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="D74" s="31" t="s">
-        <v>135</v>
+      <c r="D74" s="29" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:256">
       <c r="A75" s="12"/>
-      <c r="B75" s="56" t="s">
+      <c r="B75" s="48" t="s">
         <v>134</v>
       </c>
       <c r="C75" s="48" t="s">
         <v>101</v>
       </c>
       <c r="D75" s="29" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76" spans="1:256">
@@ -5498,20 +5501,273 @@
         <v>101</v>
       </c>
       <c r="D76" s="29" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:256">
       <c r="A77" s="12"/>
-      <c r="B77" s="48" t="s">
-        <v>134</v>
-      </c>
-      <c r="C77" s="48" t="s">
-        <v>101</v>
+      <c r="B77" s="48" t="str">
+        <f>ReactionList!A36</f>
+        <v>eIF4E_[A001]_ppi+_EIF4EBP1_[A001]</v>
+      </c>
+      <c r="C77" s="45" t="s">
+        <v>87</v>
       </c>
       <c r="D77" s="29" t="s">
-        <v>138</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+      <c r="M77" s="6"/>
+      <c r="N77" s="6"/>
+      <c r="O77" s="6"/>
+      <c r="P77" s="6"/>
+      <c r="Q77" s="6"/>
+      <c r="R77" s="6"/>
+      <c r="S77" s="6"/>
+      <c r="T77" s="6"/>
+      <c r="U77" s="6"/>
+      <c r="V77" s="6"/>
+      <c r="W77" s="6"/>
+      <c r="X77" s="6"/>
+      <c r="Y77" s="6"/>
+      <c r="Z77" s="6"/>
+      <c r="AA77" s="6"/>
+      <c r="AB77" s="6"/>
+      <c r="AC77" s="6"/>
+      <c r="AD77" s="6"/>
+      <c r="AE77" s="6"/>
+      <c r="AF77" s="6"/>
+      <c r="AG77" s="6"/>
+      <c r="AH77" s="6"/>
+      <c r="AI77" s="6"/>
+      <c r="AJ77" s="6"/>
+      <c r="AK77" s="6"/>
+      <c r="AL77" s="6"/>
+      <c r="AM77" s="6"/>
+      <c r="AN77" s="6"/>
+      <c r="AO77" s="6"/>
+      <c r="AP77" s="6"/>
+      <c r="AQ77" s="6"/>
+      <c r="AR77" s="6"/>
+      <c r="AS77" s="6"/>
+      <c r="AT77" s="6"/>
+      <c r="AU77" s="6"/>
+      <c r="AV77" s="6"/>
+      <c r="AW77" s="6"/>
+      <c r="AX77" s="6"/>
+      <c r="AY77" s="6"/>
+      <c r="AZ77" s="6"/>
+      <c r="BA77" s="6"/>
+      <c r="BB77" s="6"/>
+      <c r="BC77" s="6"/>
+      <c r="BD77" s="6"/>
+      <c r="BE77" s="6"/>
+      <c r="BF77" s="6"/>
+      <c r="BG77" s="6"/>
+      <c r="BH77" s="6"/>
+      <c r="BI77" s="6"/>
+      <c r="BJ77" s="6"/>
+      <c r="BK77" s="6"/>
+      <c r="BL77" s="6"/>
+      <c r="BM77" s="6"/>
+      <c r="BN77" s="6"/>
+      <c r="BO77" s="6"/>
+      <c r="BP77" s="6"/>
+      <c r="BQ77" s="6"/>
+      <c r="BR77" s="6"/>
+      <c r="BS77" s="6"/>
+      <c r="BT77" s="6"/>
+      <c r="BU77" s="6"/>
+      <c r="BV77" s="6"/>
+      <c r="BW77" s="6"/>
+      <c r="BX77" s="6"/>
+      <c r="BY77" s="6"/>
+      <c r="BZ77" s="6"/>
+      <c r="CA77" s="6"/>
+      <c r="CB77" s="6"/>
+      <c r="CC77" s="6"/>
+      <c r="CD77" s="6"/>
+      <c r="CE77" s="6"/>
+      <c r="CF77" s="6"/>
+      <c r="CG77" s="6"/>
+      <c r="CH77" s="6"/>
+      <c r="CI77" s="6"/>
+      <c r="CJ77" s="6"/>
+      <c r="CK77" s="6"/>
+      <c r="CL77" s="6"/>
+      <c r="CM77" s="6"/>
+      <c r="CN77" s="6"/>
+      <c r="CO77" s="6"/>
+      <c r="CP77" s="6"/>
+      <c r="CQ77" s="6"/>
+      <c r="CR77" s="6"/>
+      <c r="CS77" s="6"/>
+      <c r="CT77" s="6"/>
+      <c r="CU77" s="6"/>
+      <c r="CV77" s="6"/>
+      <c r="CW77" s="6"/>
+      <c r="CX77" s="6"/>
+      <c r="CY77" s="6"/>
+      <c r="CZ77" s="6"/>
+      <c r="DA77" s="6"/>
+      <c r="DB77" s="6"/>
+      <c r="DC77" s="6"/>
+      <c r="DD77" s="6"/>
+      <c r="DE77" s="6"/>
+      <c r="DF77" s="6"/>
+      <c r="DG77" s="6"/>
+      <c r="DH77" s="6"/>
+      <c r="DI77" s="6"/>
+      <c r="DJ77" s="6"/>
+      <c r="DK77" s="6"/>
+      <c r="DL77" s="6"/>
+      <c r="DM77" s="6"/>
+      <c r="DN77" s="6"/>
+      <c r="DO77" s="6"/>
+      <c r="DP77" s="6"/>
+      <c r="DQ77" s="6"/>
+      <c r="DR77" s="6"/>
+      <c r="DS77" s="6"/>
+      <c r="DT77" s="6"/>
+      <c r="DU77" s="6"/>
+      <c r="DV77" s="6"/>
+      <c r="DW77" s="6"/>
+      <c r="DX77" s="6"/>
+      <c r="DY77" s="6"/>
+      <c r="DZ77" s="6"/>
+      <c r="EA77" s="6"/>
+      <c r="EB77" s="6"/>
+      <c r="EC77" s="6"/>
+      <c r="ED77" s="6"/>
+      <c r="EE77" s="6"/>
+      <c r="EF77" s="6"/>
+      <c r="EG77" s="6"/>
+      <c r="EH77" s="6"/>
+      <c r="EI77" s="6"/>
+      <c r="EJ77" s="6"/>
+      <c r="EK77" s="6"/>
+      <c r="EL77" s="6"/>
+      <c r="EM77" s="6"/>
+      <c r="EN77" s="6"/>
+      <c r="EO77" s="6"/>
+      <c r="EP77" s="6"/>
+      <c r="EQ77" s="6"/>
+      <c r="ER77" s="6"/>
+      <c r="ES77" s="6"/>
+      <c r="ET77" s="6"/>
+      <c r="EU77" s="6"/>
+      <c r="EV77" s="6"/>
+      <c r="EW77" s="6"/>
+      <c r="EX77" s="6"/>
+      <c r="EY77" s="6"/>
+      <c r="EZ77" s="6"/>
+      <c r="FA77" s="6"/>
+      <c r="FB77" s="6"/>
+      <c r="FC77" s="6"/>
+      <c r="FD77" s="6"/>
+      <c r="FE77" s="6"/>
+      <c r="FF77" s="6"/>
+      <c r="FG77" s="6"/>
+      <c r="FH77" s="6"/>
+      <c r="FI77" s="6"/>
+      <c r="FJ77" s="6"/>
+      <c r="FK77" s="6"/>
+      <c r="FL77" s="6"/>
+      <c r="FM77" s="6"/>
+      <c r="FN77" s="6"/>
+      <c r="FO77" s="6"/>
+      <c r="FP77" s="6"/>
+      <c r="FQ77" s="6"/>
+      <c r="FR77" s="6"/>
+      <c r="FS77" s="6"/>
+      <c r="FT77" s="6"/>
+      <c r="FU77" s="6"/>
+      <c r="FV77" s="6"/>
+      <c r="FW77" s="6"/>
+      <c r="FX77" s="6"/>
+      <c r="FY77" s="6"/>
+      <c r="FZ77" s="6"/>
+      <c r="GA77" s="6"/>
+      <c r="GB77" s="6"/>
+      <c r="GC77" s="6"/>
+      <c r="GD77" s="6"/>
+      <c r="GE77" s="6"/>
+      <c r="GF77" s="6"/>
+      <c r="GG77" s="6"/>
+      <c r="GH77" s="6"/>
+      <c r="GI77" s="6"/>
+      <c r="GJ77" s="6"/>
+      <c r="GK77" s="6"/>
+      <c r="GL77" s="6"/>
+      <c r="GM77" s="6"/>
+      <c r="GN77" s="6"/>
+      <c r="GO77" s="6"/>
+      <c r="GP77" s="6"/>
+      <c r="GQ77" s="6"/>
+      <c r="GR77" s="6"/>
+      <c r="GS77" s="6"/>
+      <c r="GT77" s="6"/>
+      <c r="GU77" s="6"/>
+      <c r="GV77" s="6"/>
+      <c r="GW77" s="6"/>
+      <c r="GX77" s="6"/>
+      <c r="GY77" s="6"/>
+      <c r="GZ77" s="6"/>
+      <c r="HA77" s="6"/>
+      <c r="HB77" s="6"/>
+      <c r="HC77" s="6"/>
+      <c r="HD77" s="6"/>
+      <c r="HE77" s="6"/>
+      <c r="HF77" s="6"/>
+      <c r="HG77" s="6"/>
+      <c r="HH77" s="6"/>
+      <c r="HI77" s="6"/>
+      <c r="HJ77" s="6"/>
+      <c r="HK77" s="6"/>
+      <c r="HL77" s="6"/>
+      <c r="HM77" s="6"/>
+      <c r="HN77" s="6"/>
+      <c r="HO77" s="6"/>
+      <c r="HP77" s="6"/>
+      <c r="HQ77" s="6"/>
+      <c r="HR77" s="6"/>
+      <c r="HS77" s="6"/>
+      <c r="HT77" s="6"/>
+      <c r="HU77" s="6"/>
+      <c r="HV77" s="6"/>
+      <c r="HW77" s="6"/>
+      <c r="HX77" s="6"/>
+      <c r="HY77" s="6"/>
+      <c r="HZ77" s="6"/>
+      <c r="IA77" s="6"/>
+      <c r="IB77" s="6"/>
+      <c r="IC77" s="6"/>
+      <c r="ID77" s="6"/>
+      <c r="IE77" s="6"/>
+      <c r="IF77" s="6"/>
+      <c r="IG77" s="6"/>
+      <c r="IH77" s="6"/>
+      <c r="II77" s="6"/>
+      <c r="IJ77" s="6"/>
+      <c r="IK77" s="6"/>
+      <c r="IL77" s="6"/>
+      <c r="IM77" s="6"/>
+      <c r="IN77" s="6"/>
+      <c r="IO77" s="6"/>
+      <c r="IP77" s="6"/>
+      <c r="IQ77" s="6"/>
+      <c r="IR77" s="6"/>
+      <c r="IS77" s="6"/>
+      <c r="IT77" s="6"/>
+      <c r="IU77" s="6"/>
+      <c r="IV77" s="6"/>
     </row>
     <row r="78" spans="1:256">
       <c r="A78" s="12"/>
@@ -5523,7 +5779,7 @@
         <v>87</v>
       </c>
       <c r="D78" s="29" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
@@ -5781,14 +6037,14 @@
     <row r="79" spans="1:256">
       <c r="A79" s="12"/>
       <c r="B79" s="48" t="str">
-        <f>ReactionList!A36</f>
-        <v>eIF4E_[A001]_ppi+_EIF4EBP1_[A001]</v>
-      </c>
-      <c r="C79" s="45" t="s">
+        <f>ReactionList!A46</f>
+        <v>eIF4E_[A001]_ppi_eIF4G_[A002]</v>
+      </c>
+      <c r="C79" s="54" t="s">
         <v>87</v>
       </c>
       <c r="D79" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E79" s="6"/>
       <c r="F79" s="6"/>
@@ -6049,11 +6305,11 @@
         <f>ReactionList!A46</f>
         <v>eIF4E_[A001]_ppi_eIF4G_[A002]</v>
       </c>
-      <c r="C80" s="54" t="s">
+      <c r="C80" s="45" t="s">
         <v>87</v>
       </c>
       <c r="D80" s="29" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
@@ -6308,333 +6564,71 @@
       <c r="IU80" s="6"/>
       <c r="IV80" s="6"/>
     </row>
-    <row r="81" spans="1:256">
+    <row r="81" spans="1:4">
       <c r="A81" s="12"/>
       <c r="B81" s="48" t="str">
         <f>ReactionList!A46</f>
         <v>eIF4E_[A001]_ppi_eIF4G_[A002]</v>
       </c>
-      <c r="C81" s="45" t="s">
+      <c r="C81" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="D81" s="29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="12"/>
+      <c r="B82" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="C82" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="D81" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
-      <c r="G81" s="6"/>
-      <c r="H81" s="6"/>
-      <c r="I81" s="6"/>
-      <c r="J81" s="6"/>
-      <c r="K81" s="6"/>
-      <c r="L81" s="6"/>
-      <c r="M81" s="6"/>
-      <c r="N81" s="6"/>
-      <c r="O81" s="6"/>
-      <c r="P81" s="6"/>
-      <c r="Q81" s="6"/>
-      <c r="R81" s="6"/>
-      <c r="S81" s="6"/>
-      <c r="T81" s="6"/>
-      <c r="U81" s="6"/>
-      <c r="V81" s="6"/>
-      <c r="W81" s="6"/>
-      <c r="X81" s="6"/>
-      <c r="Y81" s="6"/>
-      <c r="Z81" s="6"/>
-      <c r="AA81" s="6"/>
-      <c r="AB81" s="6"/>
-      <c r="AC81" s="6"/>
-      <c r="AD81" s="6"/>
-      <c r="AE81" s="6"/>
-      <c r="AF81" s="6"/>
-      <c r="AG81" s="6"/>
-      <c r="AH81" s="6"/>
-      <c r="AI81" s="6"/>
-      <c r="AJ81" s="6"/>
-      <c r="AK81" s="6"/>
-      <c r="AL81" s="6"/>
-      <c r="AM81" s="6"/>
-      <c r="AN81" s="6"/>
-      <c r="AO81" s="6"/>
-      <c r="AP81" s="6"/>
-      <c r="AQ81" s="6"/>
-      <c r="AR81" s="6"/>
-      <c r="AS81" s="6"/>
-      <c r="AT81" s="6"/>
-      <c r="AU81" s="6"/>
-      <c r="AV81" s="6"/>
-      <c r="AW81" s="6"/>
-      <c r="AX81" s="6"/>
-      <c r="AY81" s="6"/>
-      <c r="AZ81" s="6"/>
-      <c r="BA81" s="6"/>
-      <c r="BB81" s="6"/>
-      <c r="BC81" s="6"/>
-      <c r="BD81" s="6"/>
-      <c r="BE81" s="6"/>
-      <c r="BF81" s="6"/>
-      <c r="BG81" s="6"/>
-      <c r="BH81" s="6"/>
-      <c r="BI81" s="6"/>
-      <c r="BJ81" s="6"/>
-      <c r="BK81" s="6"/>
-      <c r="BL81" s="6"/>
-      <c r="BM81" s="6"/>
-      <c r="BN81" s="6"/>
-      <c r="BO81" s="6"/>
-      <c r="BP81" s="6"/>
-      <c r="BQ81" s="6"/>
-      <c r="BR81" s="6"/>
-      <c r="BS81" s="6"/>
-      <c r="BT81" s="6"/>
-      <c r="BU81" s="6"/>
-      <c r="BV81" s="6"/>
-      <c r="BW81" s="6"/>
-      <c r="BX81" s="6"/>
-      <c r="BY81" s="6"/>
-      <c r="BZ81" s="6"/>
-      <c r="CA81" s="6"/>
-      <c r="CB81" s="6"/>
-      <c r="CC81" s="6"/>
-      <c r="CD81" s="6"/>
-      <c r="CE81" s="6"/>
-      <c r="CF81" s="6"/>
-      <c r="CG81" s="6"/>
-      <c r="CH81" s="6"/>
-      <c r="CI81" s="6"/>
-      <c r="CJ81" s="6"/>
-      <c r="CK81" s="6"/>
-      <c r="CL81" s="6"/>
-      <c r="CM81" s="6"/>
-      <c r="CN81" s="6"/>
-      <c r="CO81" s="6"/>
-      <c r="CP81" s="6"/>
-      <c r="CQ81" s="6"/>
-      <c r="CR81" s="6"/>
-      <c r="CS81" s="6"/>
-      <c r="CT81" s="6"/>
-      <c r="CU81" s="6"/>
-      <c r="CV81" s="6"/>
-      <c r="CW81" s="6"/>
-      <c r="CX81" s="6"/>
-      <c r="CY81" s="6"/>
-      <c r="CZ81" s="6"/>
-      <c r="DA81" s="6"/>
-      <c r="DB81" s="6"/>
-      <c r="DC81" s="6"/>
-      <c r="DD81" s="6"/>
-      <c r="DE81" s="6"/>
-      <c r="DF81" s="6"/>
-      <c r="DG81" s="6"/>
-      <c r="DH81" s="6"/>
-      <c r="DI81" s="6"/>
-      <c r="DJ81" s="6"/>
-      <c r="DK81" s="6"/>
-      <c r="DL81" s="6"/>
-      <c r="DM81" s="6"/>
-      <c r="DN81" s="6"/>
-      <c r="DO81" s="6"/>
-      <c r="DP81" s="6"/>
-      <c r="DQ81" s="6"/>
-      <c r="DR81" s="6"/>
-      <c r="DS81" s="6"/>
-      <c r="DT81" s="6"/>
-      <c r="DU81" s="6"/>
-      <c r="DV81" s="6"/>
-      <c r="DW81" s="6"/>
-      <c r="DX81" s="6"/>
-      <c r="DY81" s="6"/>
-      <c r="DZ81" s="6"/>
-      <c r="EA81" s="6"/>
-      <c r="EB81" s="6"/>
-      <c r="EC81" s="6"/>
-      <c r="ED81" s="6"/>
-      <c r="EE81" s="6"/>
-      <c r="EF81" s="6"/>
-      <c r="EG81" s="6"/>
-      <c r="EH81" s="6"/>
-      <c r="EI81" s="6"/>
-      <c r="EJ81" s="6"/>
-      <c r="EK81" s="6"/>
-      <c r="EL81" s="6"/>
-      <c r="EM81" s="6"/>
-      <c r="EN81" s="6"/>
-      <c r="EO81" s="6"/>
-      <c r="EP81" s="6"/>
-      <c r="EQ81" s="6"/>
-      <c r="ER81" s="6"/>
-      <c r="ES81" s="6"/>
-      <c r="ET81" s="6"/>
-      <c r="EU81" s="6"/>
-      <c r="EV81" s="6"/>
-      <c r="EW81" s="6"/>
-      <c r="EX81" s="6"/>
-      <c r="EY81" s="6"/>
-      <c r="EZ81" s="6"/>
-      <c r="FA81" s="6"/>
-      <c r="FB81" s="6"/>
-      <c r="FC81" s="6"/>
-      <c r="FD81" s="6"/>
-      <c r="FE81" s="6"/>
-      <c r="FF81" s="6"/>
-      <c r="FG81" s="6"/>
-      <c r="FH81" s="6"/>
-      <c r="FI81" s="6"/>
-      <c r="FJ81" s="6"/>
-      <c r="FK81" s="6"/>
-      <c r="FL81" s="6"/>
-      <c r="FM81" s="6"/>
-      <c r="FN81" s="6"/>
-      <c r="FO81" s="6"/>
-      <c r="FP81" s="6"/>
-      <c r="FQ81" s="6"/>
-      <c r="FR81" s="6"/>
-      <c r="FS81" s="6"/>
-      <c r="FT81" s="6"/>
-      <c r="FU81" s="6"/>
-      <c r="FV81" s="6"/>
-      <c r="FW81" s="6"/>
-      <c r="FX81" s="6"/>
-      <c r="FY81" s="6"/>
-      <c r="FZ81" s="6"/>
-      <c r="GA81" s="6"/>
-      <c r="GB81" s="6"/>
-      <c r="GC81" s="6"/>
-      <c r="GD81" s="6"/>
-      <c r="GE81" s="6"/>
-      <c r="GF81" s="6"/>
-      <c r="GG81" s="6"/>
-      <c r="GH81" s="6"/>
-      <c r="GI81" s="6"/>
-      <c r="GJ81" s="6"/>
-      <c r="GK81" s="6"/>
-      <c r="GL81" s="6"/>
-      <c r="GM81" s="6"/>
-      <c r="GN81" s="6"/>
-      <c r="GO81" s="6"/>
-      <c r="GP81" s="6"/>
-      <c r="GQ81" s="6"/>
-      <c r="GR81" s="6"/>
-      <c r="GS81" s="6"/>
-      <c r="GT81" s="6"/>
-      <c r="GU81" s="6"/>
-      <c r="GV81" s="6"/>
-      <c r="GW81" s="6"/>
-      <c r="GX81" s="6"/>
-      <c r="GY81" s="6"/>
-      <c r="GZ81" s="6"/>
-      <c r="HA81" s="6"/>
-      <c r="HB81" s="6"/>
-      <c r="HC81" s="6"/>
-      <c r="HD81" s="6"/>
-      <c r="HE81" s="6"/>
-      <c r="HF81" s="6"/>
-      <c r="HG81" s="6"/>
-      <c r="HH81" s="6"/>
-      <c r="HI81" s="6"/>
-      <c r="HJ81" s="6"/>
-      <c r="HK81" s="6"/>
-      <c r="HL81" s="6"/>
-      <c r="HM81" s="6"/>
-      <c r="HN81" s="6"/>
-      <c r="HO81" s="6"/>
-      <c r="HP81" s="6"/>
-      <c r="HQ81" s="6"/>
-      <c r="HR81" s="6"/>
-      <c r="HS81" s="6"/>
-      <c r="HT81" s="6"/>
-      <c r="HU81" s="6"/>
-      <c r="HV81" s="6"/>
-      <c r="HW81" s="6"/>
-      <c r="HX81" s="6"/>
-      <c r="HY81" s="6"/>
-      <c r="HZ81" s="6"/>
-      <c r="IA81" s="6"/>
-      <c r="IB81" s="6"/>
-      <c r="IC81" s="6"/>
-      <c r="ID81" s="6"/>
-      <c r="IE81" s="6"/>
-      <c r="IF81" s="6"/>
-      <c r="IG81" s="6"/>
-      <c r="IH81" s="6"/>
-      <c r="II81" s="6"/>
-      <c r="IJ81" s="6"/>
-      <c r="IK81" s="6"/>
-      <c r="IL81" s="6"/>
-      <c r="IM81" s="6"/>
-      <c r="IN81" s="6"/>
-      <c r="IO81" s="6"/>
-      <c r="IP81" s="6"/>
-      <c r="IQ81" s="6"/>
-      <c r="IR81" s="6"/>
-      <c r="IS81" s="6"/>
-      <c r="IT81" s="6"/>
-      <c r="IU81" s="6"/>
-      <c r="IV81" s="6"/>
-    </row>
-    <row r="82" spans="1:256">
-      <c r="A82" s="12"/>
-      <c r="B82" s="48" t="str">
-        <f>ReactionList!A46</f>
-        <v>eIF4E_[A001]_ppi_eIF4G_[A002]</v>
-      </c>
-      <c r="C82" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="D82" s="29" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="83" spans="1:256">
+      <c r="D82" s="47" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" s="12"/>
-      <c r="B83" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="C83" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="D83" s="47" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="84" spans="1:256">
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" s="12"/>
     </row>
-    <row r="85" spans="1:256">
+    <row r="85" spans="1:4">
       <c r="A85" s="12"/>
     </row>
-    <row r="86" spans="1:256">
+    <row r="86" spans="1:4">
       <c r="A86" s="12"/>
     </row>
-    <row r="87" spans="1:256">
+    <row r="87" spans="1:4">
       <c r="A87" s="12"/>
     </row>
-    <row r="88" spans="1:256">
+    <row r="88" spans="1:4">
       <c r="A88" s="12"/>
     </row>
-    <row r="89" spans="1:256">
+    <row r="89" spans="1:4">
       <c r="A89" s="12"/>
     </row>
-    <row r="90" spans="1:256">
+    <row r="90" spans="1:4">
       <c r="A90" s="12"/>
     </row>
-    <row r="91" spans="1:256">
+    <row r="91" spans="1:4">
       <c r="A91" s="12"/>
     </row>
-    <row r="92" spans="1:256">
+    <row r="92" spans="1:4">
       <c r="A92" s="12"/>
     </row>
-    <row r="93" spans="1:256">
+    <row r="93" spans="1:4">
       <c r="A93" s="12"/>
     </row>
-    <row r="94" spans="1:256">
+    <row r="94" spans="1:4">
       <c r="A94" s="12"/>
     </row>
-    <row r="95" spans="1:256">
+    <row r="95" spans="1:4">
       <c r="A95" s="12"/>
     </row>
-    <row r="96" spans="1:256">
+    <row r="96" spans="1:4">
       <c r="A96" s="12"/>
     </row>
     <row r="97" spans="1:1">
@@ -6793,29 +6787,26 @@
     <row r="148" spans="1:1">
       <c r="A148" s="12"/>
     </row>
-    <row r="149" spans="1:1">
-      <c r="A149" s="12"/>
-    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <conditionalFormatting sqref="D49 B31:B39">
+  <conditionalFormatting sqref="D48 B30:B38">
     <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
-      <formula>NOT(ISERROR(SEARCH("Error",B31)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Error",B30)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H64852:H64862 E72:H83 C72:C83 C67 B84:H149 A150:H64851 H27:H71 H2:H24">
+  <conditionalFormatting sqref="H64851:H64861 E71:H82 C71:C82 C66 B83:H148 A149:H64850 H26:H70 H2:H23">
     <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>ISERROR(A2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H25:H26">
+  <conditionalFormatting sqref="H24:H25">
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>ISERROR(H25)</formula>
+      <formula>ISERROR(H24)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E59">
+  <conditionalFormatting sqref="E58">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>NOT(ISERROR(SEARCH("Error",E59)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Error",E58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>

</xml_diff>